<commit_message>
Refactor: Sistema Asistencia Backend - Modificaion main.py
</commit_message>
<xml_diff>
--- a/sistema-asistencia-backend/lista_cooperativistas_agosto.xlsx
+++ b/sistema-asistencia-backend/lista_cooperativistas_agosto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Desktop\Sistema-Asistencia\sistema-asistencia-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550A85E2-1475-4C5F-B085-C73CA0F7D6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977ACAD3-EC8D-4303-8651-BCC9785B994B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C65746CC-08ED-4377-91D0-9F16FFE7E6FB}"/>
   </bookViews>
@@ -5804,8 +5804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769E6F53-B82A-4984-B2ED-7A38B7865E3F}">
   <dimension ref="A1:O894"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A475" workbookViewId="0">
-      <selection activeCell="A390" sqref="A390:XFD390"/>
+    <sheetView tabSelected="1" topLeftCell="A750" workbookViewId="0">
+      <selection activeCell="J764" sqref="J764"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34512,9 +34512,6 @@
       <c r="I764" t="s">
         <v>1569</v>
       </c>
-      <c r="J764">
-        <v>4078163</v>
-      </c>
       <c r="K764" s="3">
         <v>45413</v>
       </c>

</xml_diff>